<commit_message>
user login and profile management
</commit_message>
<xml_diff>
--- a/test/resources/unittest_DAZHO_1_74_2024_2023.xlsx
+++ b/test/resources/unittest_DAZHO_1_74_2024_2023.xlsx
@@ -295,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
@@ -464,18 +464,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1978,18 +1966,18 @@
       <c r="AC23" s="1" t="n"/>
     </row>
     <row r="24" ht="16" customHeight="1">
-      <c r="A24" s="60" t="inlineStr">
+      <c r="A24" s="47" t="inlineStr">
         <is>
           <t>16а</t>
         </is>
       </c>
-      <c r="B24" s="61" t="inlineStr"/>
-      <c r="C24" s="62" t="inlineStr"/>
+      <c r="B24" s="48" t="inlineStr"/>
+      <c r="C24" s="49" t="inlineStr"/>
       <c r="D24" s="50" t="inlineStr"/>
       <c r="E24" s="50" t="inlineStr"/>
       <c r="F24" s="50" t="inlineStr"/>
       <c r="G24" s="50" t="inlineStr"/>
-      <c r="H24" s="63" t="inlineStr">
+      <c r="H24" s="46" t="inlineStr">
         <is>
           <t>unlinked</t>
         </is>
@@ -3392,7 +3380,7 @@
           <t>Метричні книги православні</t>
         </is>
       </c>
-      <c r="C55" s="64" t="inlineStr">
+      <c r="C55" s="60" t="inlineStr">
         <is>
           <t>1801</t>
         </is>
@@ -4790,17 +4778,17 @@
       <c r="N98" s="50" t="inlineStr"/>
     </row>
     <row r="99">
-      <c r="A99" s="60" t="inlineStr">
+      <c r="A99" s="47" t="inlineStr">
         <is>
           <t>90а</t>
         </is>
       </c>
-      <c r="B99" s="61" t="inlineStr">
-        <is>
-          <t>Метричні книги православні</t>
-        </is>
-      </c>
-      <c r="C99" s="62" t="inlineStr">
+      <c r="B99" s="48" t="inlineStr">
+        <is>
+          <t>Метричні книги православні</t>
+        </is>
+      </c>
+      <c r="C99" s="49" t="inlineStr">
         <is>
           <t>1839</t>
         </is>
@@ -4809,7 +4797,7 @@
       <c r="E99" s="50" t="inlineStr"/>
       <c r="F99" s="50" t="inlineStr"/>
       <c r="G99" s="50" t="inlineStr"/>
-      <c r="H99" s="63" t="inlineStr">
+      <c r="H99" s="46" t="inlineStr">
         <is>
           <t>linked</t>
         </is>
@@ -5270,17 +5258,17 @@
       <c r="N113" s="50" t="inlineStr"/>
     </row>
     <row r="114">
-      <c r="A114" s="60" t="inlineStr">
+      <c r="A114" s="47" t="inlineStr">
         <is>
           <t>104а</t>
         </is>
       </c>
-      <c r="B114" s="61" t="inlineStr">
-        <is>
-          <t>Метричні книги православні</t>
-        </is>
-      </c>
-      <c r="C114" s="62" t="inlineStr">
+      <c r="B114" s="48" t="inlineStr">
+        <is>
+          <t>Метричні книги православні</t>
+        </is>
+      </c>
+      <c r="C114" s="49" t="inlineStr">
         <is>
           <t>1846</t>
         </is>
@@ -5289,7 +5277,7 @@
       <c r="E114" s="50" t="inlineStr"/>
       <c r="F114" s="50" t="inlineStr"/>
       <c r="G114" s="50" t="inlineStr"/>
-      <c r="H114" s="63" t="inlineStr">
+      <c r="H114" s="46" t="inlineStr">
         <is>
           <t>unlinked</t>
         </is>
@@ -7798,17 +7786,17 @@
       <c r="N192" s="50" t="inlineStr"/>
     </row>
     <row r="193">
-      <c r="A193" s="60" t="inlineStr">
+      <c r="A193" s="47" t="inlineStr">
         <is>
           <t>183а</t>
         </is>
       </c>
-      <c r="B193" s="61" t="inlineStr">
+      <c r="B193" s="48" t="inlineStr">
         <is>
           <t>Метричні книги православні (народження)</t>
         </is>
       </c>
-      <c r="C193" s="62" t="inlineStr">
+      <c r="C193" s="49" t="inlineStr">
         <is>
           <t>1832</t>
         </is>
@@ -7817,7 +7805,7 @@
       <c r="E193" s="50" t="inlineStr"/>
       <c r="F193" s="50" t="inlineStr"/>
       <c r="G193" s="50" t="inlineStr"/>
-      <c r="H193" s="63" t="inlineStr">
+      <c r="H193" s="46" t="inlineStr">
         <is>
           <t>unlinked</t>
         </is>
@@ -7899,7 +7887,7 @@
           <t>186</t>
         </is>
       </c>
-      <c r="B196" s="65" t="inlineStr">
+      <c r="B196" s="61" t="inlineStr">
         <is>
           <t>Сповідні списки православні А-Ж</t>
         </is>
@@ -7931,7 +7919,7 @@
           <t>187</t>
         </is>
       </c>
-      <c r="B197" s="65" t="inlineStr">
+      <c r="B197" s="61" t="inlineStr">
         <is>
           <t>Сповідні списки православні З-О</t>
         </is>
@@ -7963,7 +7951,7 @@
           <t>188</t>
         </is>
       </c>
-      <c r="B198" s="65" t="inlineStr">
+      <c r="B198" s="61" t="inlineStr">
         <is>
           <t>Сповідні списки православні П-Я</t>
         </is>
@@ -8182,17 +8170,17 @@
       <c r="N204" s="50" t="inlineStr"/>
     </row>
     <row r="205">
-      <c r="A205" s="60" t="inlineStr">
+      <c r="A205" s="47" t="inlineStr">
         <is>
           <t>194а</t>
         </is>
       </c>
-      <c r="B205" s="61" t="inlineStr">
+      <c r="B205" s="48" t="inlineStr">
         <is>
           <t>Метричні книги православні (смеоть)</t>
         </is>
       </c>
-      <c r="C205" s="62" t="inlineStr">
+      <c r="C205" s="49" t="inlineStr">
         <is>
           <t>1836</t>
         </is>
@@ -8201,7 +8189,7 @@
       <c r="E205" s="50" t="inlineStr"/>
       <c r="F205" s="50" t="inlineStr"/>
       <c r="G205" s="50" t="inlineStr"/>
-      <c r="H205" s="63" t="inlineStr">
+      <c r="H205" s="46" t="inlineStr">
         <is>
           <t>unlinked</t>
         </is>
@@ -8731,7 +8719,7 @@
           <t>211</t>
         </is>
       </c>
-      <c r="B222" s="65" t="inlineStr">
+      <c r="B222" s="61" t="inlineStr">
         <is>
           <t>Сповідні розписи православних церков Ровенського повіту. Села З-О.</t>
         </is>
@@ -8827,7 +8815,7 @@
           <t>214</t>
         </is>
       </c>
-      <c r="B225" s="65" t="inlineStr">
+      <c r="B225" s="61" t="inlineStr">
         <is>
           <t>Сповідні відомості православних церков Ровенського повіту. Села С-Я</t>
         </is>
@@ -9910,17 +9898,17 @@
       <c r="N258" s="50" t="inlineStr"/>
     </row>
     <row r="259">
-      <c r="A259" s="60" t="inlineStr">
+      <c r="A259" s="47" t="inlineStr">
         <is>
           <t>247а</t>
         </is>
       </c>
-      <c r="B259" s="61" t="inlineStr">
+      <c r="B259" s="48" t="inlineStr">
         <is>
           <t>Метричні книги села Калинівка (Покровська церква)</t>
         </is>
       </c>
-      <c r="C259" s="62" t="inlineStr">
+      <c r="C259" s="49" t="inlineStr">
         <is>
           <t>1821-1832</t>
         </is>
@@ -9929,7 +9917,7 @@
       <c r="E259" s="50" t="inlineStr"/>
       <c r="F259" s="50" t="inlineStr"/>
       <c r="G259" s="50" t="inlineStr"/>
-      <c r="H259" s="63" t="inlineStr">
+      <c r="H259" s="46" t="inlineStr">
         <is>
           <t>unlinked</t>
         </is>
@@ -11104,7 +11092,7 @@
           <t>Метричні книги православні</t>
         </is>
       </c>
-      <c r="C296" s="64" t="inlineStr">
+      <c r="C296" s="60" t="inlineStr">
         <is>
           <t>1373</t>
         </is>
@@ -12283,7 +12271,7 @@
           <t>321</t>
         </is>
       </c>
-      <c r="B333" s="65" t="inlineStr">
+      <c r="B333" s="61" t="inlineStr">
         <is>
           <t>Метричні книги православних церков Овруцького повіту</t>
         </is>
@@ -12411,7 +12399,7 @@
           <t>325</t>
         </is>
       </c>
-      <c r="B337" s="65" t="inlineStr">
+      <c r="B337" s="61" t="inlineStr">
         <is>
           <t>Метричні книги православних церков Овруцького повіту</t>
         </is>
@@ -13051,12 +13039,12 @@
           <t>345</t>
         </is>
       </c>
-      <c r="B357" s="65" t="inlineStr">
+      <c r="B357" s="61" t="inlineStr">
         <is>
           <t>Метричні книги православні,села Б-Л</t>
         </is>
       </c>
-      <c r="C357" s="64" t="inlineStr">
+      <c r="C357" s="60" t="inlineStr">
         <is>
           <t>1867</t>
         </is>
@@ -13179,7 +13167,7 @@
           <t>351</t>
         </is>
       </c>
-      <c r="B361" s="65" t="inlineStr">
+      <c r="B361" s="61" t="inlineStr">
         <is>
           <t>Сповідальні відомості православних церков Луцького повіту. Села Р-Я</t>
         </is>
@@ -14107,12 +14095,12 @@
           <t>406</t>
         </is>
       </c>
-      <c r="B390" s="65" t="inlineStr">
+      <c r="B390" s="61" t="inlineStr">
         <is>
           <t>Сповідальні відомості. Села О-Я</t>
         </is>
       </c>
-      <c r="C390" s="64" t="inlineStr">
+      <c r="C390" s="60" t="inlineStr">
         <is>
           <t>1912(1911)</t>
         </is>
@@ -14139,7 +14127,7 @@
           <t>407</t>
         </is>
       </c>
-      <c r="B391" s="65" t="inlineStr">
+      <c r="B391" s="61" t="inlineStr">
         <is>
           <t>Сповідальні відомості. Села З-О</t>
         </is>
@@ -14171,7 +14159,7 @@
           <t>408</t>
         </is>
       </c>
-      <c r="B392" s="65" t="inlineStr">
+      <c r="B392" s="61" t="inlineStr">
         <is>
           <t>Сповідальні відомості. Села А-З</t>
         </is>
@@ -14208,7 +14196,7 @@
           <t>Сповідальні відомості. Села Д-К</t>
         </is>
       </c>
-      <c r="C393" s="64" t="inlineStr">
+      <c r="C393" s="60" t="inlineStr">
         <is>
           <t>1913</t>
         </is>
@@ -14235,12 +14223,12 @@
           <t>410</t>
         </is>
       </c>
-      <c r="B394" s="65" t="inlineStr">
+      <c r="B394" s="61" t="inlineStr">
         <is>
           <t>Сповідальні відомості. Села А-Д</t>
         </is>
       </c>
-      <c r="C394" s="64" t="inlineStr">
+      <c r="C394" s="60" t="inlineStr">
         <is>
           <t>1913</t>
         </is>

</xml_diff>